<commit_message>
protected column 1 of the spreadsheet; column 1 is not editable
</commit_message>
<xml_diff>
--- a/src/FormatForTemplateOfScores.xlsx
+++ b/src/FormatForTemplateOfScores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harle\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B90B984B-BDD1-49EC-B3E4-9987B7EF43B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{931136F9-F080-4839-B9CD-7C2636F8F1B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -174,7 +174,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -222,6 +222,18 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -323,41 +335,59 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+      <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -579,47 +609,47 @@
   </sheetPr>
   <dimension ref="A1:C1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="C44" sqref="C44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A44" sqref="A44:B44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="36" customWidth="1"/>
-    <col min="2" max="2" width="12.5703125" customWidth="1"/>
-    <col min="3" max="3" width="106.140625" customWidth="1"/>
+    <col min="1" max="1" width="36" style="2" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="106.140625" style="2" customWidth="1"/>
     <col min="4" max="6" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="16" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="11" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="3" t="s">
@@ -630,354 +660,354 @@
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="4">
         <v>73</v>
       </c>
-      <c r="C5" s="6"/>
+      <c r="C5" s="5"/>
     </row>
     <row r="6" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6" s="4">
         <v>73</v>
       </c>
-      <c r="C6" s="6"/>
+      <c r="C6" s="5"/>
     </row>
     <row r="7" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="5">
+      <c r="B7" s="4">
         <v>75</v>
       </c>
-      <c r="C7" s="8"/>
+      <c r="C7" s="6"/>
     </row>
     <row r="8" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="5">
+      <c r="B8" s="4">
         <v>79</v>
       </c>
-      <c r="C8" s="8"/>
+      <c r="C8" s="6"/>
     </row>
     <row r="9" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="5">
+      <c r="B9" s="4">
         <v>76</v>
       </c>
-      <c r="C9" s="6"/>
+      <c r="C9" s="5"/>
     </row>
     <row r="10" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A10" s="7" t="s">
+      <c r="A10" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="5">
+      <c r="B10" s="4">
         <v>75</v>
       </c>
-      <c r="C10" s="6"/>
+      <c r="C10" s="5"/>
     </row>
     <row r="11" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A11" s="7" t="s">
+      <c r="A11" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="5">
+      <c r="B11" s="4">
         <v>96</v>
       </c>
-      <c r="C11" s="6"/>
+      <c r="C11" s="5"/>
     </row>
     <row r="12" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A12" s="7" t="s">
+      <c r="A12" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="5">
+      <c r="B12" s="4">
         <v>70</v>
       </c>
-      <c r="C12" s="6"/>
+      <c r="C12" s="5"/>
     </row>
     <row r="13" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A13" s="9" t="s">
+      <c r="A13" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="10">
+      <c r="B13" s="7">
         <v>89</v>
       </c>
-      <c r="C13" s="6"/>
+      <c r="C13" s="5"/>
     </row>
     <row r="14" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A14" s="11" t="s">
+      <c r="A14" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="10">
+      <c r="B14" s="7">
         <v>97</v>
       </c>
-      <c r="C14" s="6"/>
+      <c r="C14" s="5"/>
     </row>
     <row r="15" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A15" s="11" t="s">
+      <c r="A15" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="B15" s="10">
+      <c r="B15" s="7">
         <v>85</v>
       </c>
-      <c r="C15" s="6"/>
+      <c r="C15" s="5"/>
     </row>
     <row r="16" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A16" s="4" t="s">
+      <c r="A16" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="5">
+      <c r="B16" s="4">
         <v>79</v>
       </c>
-      <c r="C16" s="6"/>
+      <c r="C16" s="5"/>
     </row>
     <row r="17" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A17" s="7" t="s">
+      <c r="A17" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B17" s="5">
+      <c r="B17" s="4">
         <v>77</v>
       </c>
-      <c r="C17" s="6"/>
+      <c r="C17" s="5"/>
     </row>
     <row r="18" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A18" s="7" t="s">
+      <c r="A18" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B18" s="5">
+      <c r="B18" s="4">
         <v>79</v>
       </c>
-      <c r="C18" s="6"/>
+      <c r="C18" s="5"/>
     </row>
     <row r="19" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A19" s="7" t="s">
+      <c r="A19" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B19" s="5">
+      <c r="B19" s="4">
         <v>88</v>
       </c>
-      <c r="C19" s="6"/>
+      <c r="C19" s="5"/>
     </row>
     <row r="20" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A20" s="9" t="s">
+      <c r="A20" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B20" s="10">
+      <c r="B20" s="7">
         <v>81</v>
       </c>
-      <c r="C20" s="6"/>
+      <c r="C20" s="5"/>
     </row>
     <row r="21" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A21" s="11" t="s">
+      <c r="A21" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="B21" s="10">
+      <c r="B21" s="7">
         <v>82</v>
       </c>
-      <c r="C21" s="6"/>
+      <c r="C21" s="5"/>
     </row>
     <row r="22" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A22" s="11" t="s">
+      <c r="A22" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="B22" s="10">
+      <c r="B22" s="7">
         <v>85</v>
       </c>
-      <c r="C22" s="6"/>
+      <c r="C22" s="5"/>
     </row>
     <row r="23" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A23" s="4" t="s">
+      <c r="A23" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="B23" s="5">
+      <c r="B23" s="4">
         <v>86</v>
       </c>
-      <c r="C23" s="6"/>
+      <c r="C23" s="5"/>
     </row>
     <row r="24" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A24" s="9" t="s">
+      <c r="A24" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="B24" s="10">
+      <c r="B24" s="7">
         <v>101</v>
       </c>
-      <c r="C24" s="6"/>
+      <c r="C24" s="5"/>
     </row>
     <row r="25" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A25" s="11" t="s">
+      <c r="A25" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="B25" s="10">
+      <c r="B25" s="7">
         <v>134</v>
       </c>
-      <c r="C25" s="6"/>
+      <c r="C25" s="5"/>
     </row>
     <row r="26" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A26" s="11" t="s">
+      <c r="A26" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="B26" s="10">
+      <c r="B26" s="7">
         <v>93</v>
       </c>
-      <c r="C26" s="6"/>
+      <c r="C26" s="5"/>
     </row>
     <row r="27" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A27" s="4" t="s">
+      <c r="A27" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="B27" s="5">
+      <c r="B27" s="4">
         <v>80</v>
       </c>
-      <c r="C27" s="6"/>
+      <c r="C27" s="5"/>
     </row>
     <row r="28" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A28" s="7" t="s">
+      <c r="A28" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="B28" s="5">
+      <c r="B28" s="4">
         <v>92</v>
       </c>
-      <c r="C28" s="6"/>
+      <c r="C28" s="5"/>
     </row>
     <row r="29" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A29" s="7" t="s">
+      <c r="A29" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="B29" s="5">
+      <c r="B29" s="4">
         <v>81</v>
       </c>
-      <c r="C29" s="6"/>
+      <c r="C29" s="5"/>
     </row>
     <row r="30" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A30" s="4" t="s">
+      <c r="A30" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="B30" s="5">
+      <c r="B30" s="4">
         <v>92</v>
       </c>
-      <c r="C30" s="6"/>
+      <c r="C30" s="5"/>
     </row>
     <row r="31" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A31" s="7" t="s">
+      <c r="A31" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="B31" s="5">
+      <c r="B31" s="4">
         <v>93</v>
       </c>
-      <c r="C31" s="6"/>
+      <c r="C31" s="5"/>
     </row>
     <row r="32" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A32" s="7" t="s">
+      <c r="A32" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="B32" s="5">
+      <c r="B32" s="4">
         <v>95</v>
       </c>
-      <c r="C32" s="6"/>
+      <c r="C32" s="5"/>
     </row>
     <row r="33" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A33" s="9" t="s">
+      <c r="A33" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="B33" s="10" t="s">
+      <c r="B33" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="C33" s="6"/>
+      <c r="C33" s="5"/>
     </row>
     <row r="34" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A34" s="11" t="s">
+      <c r="A34" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="B34" s="10" t="s">
+      <c r="B34" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="C34" s="6"/>
+      <c r="C34" s="5"/>
     </row>
     <row r="35" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A35" s="11" t="s">
+      <c r="A35" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="B35" s="10">
+      <c r="B35" s="7">
         <v>82</v>
       </c>
-      <c r="C35" s="6"/>
+      <c r="C35" s="5"/>
     </row>
     <row r="36" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A36" s="4" t="s">
+      <c r="A36" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="B36" s="5">
+      <c r="B36" s="4">
         <v>67</v>
       </c>
-      <c r="C36" s="6"/>
+      <c r="C36" s="5"/>
     </row>
     <row r="37" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A37" s="7" t="s">
+      <c r="A37" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="B37" s="5">
+      <c r="B37" s="4">
         <v>68</v>
       </c>
-      <c r="C37" s="6"/>
+      <c r="C37" s="5"/>
     </row>
     <row r="38" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A38" s="7" t="s">
+      <c r="A38" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="B38" s="5">
+      <c r="B38" s="4">
         <v>71</v>
       </c>
-      <c r="C38" s="6"/>
+      <c r="C38" s="5"/>
     </row>
     <row r="39" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A39" s="9" t="s">
+      <c r="A39" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="B39" s="10">
+      <c r="B39" s="7">
         <v>70</v>
       </c>
-      <c r="C39" s="6"/>
+      <c r="C39" s="5"/>
     </row>
     <row r="40" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A40" s="11" t="s">
+      <c r="A40" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="B40" s="10">
+      <c r="B40" s="7">
         <v>76</v>
       </c>
-      <c r="C40" s="6"/>
+      <c r="C40" s="5"/>
     </row>
     <row r="41" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A41" s="11" t="s">
+      <c r="A41" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="B41" s="10">
+      <c r="B41" s="7">
         <v>71</v>
       </c>
-      <c r="C41" s="6"/>
+      <c r="C41" s="5"/>
     </row>
     <row r="42" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A42" s="11" t="s">
+      <c r="A42" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="B42" s="10">
+      <c r="B42" s="7">
         <v>72</v>
       </c>
-      <c r="C42" s="6"/>
+      <c r="C42" s="5"/>
     </row>
     <row r="43" spans="1:3" ht="15.75" customHeight="1"/>
     <row r="44" spans="1:3" ht="185.25" customHeight="1">
-      <c r="A44" s="12" t="s">
+      <c r="A44" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="B44" s="13"/>
-      <c r="C44" s="8" t="s">
+      <c r="B44" s="9"/>
+      <c r="C44" s="17" t="s">
         <v>47</v>
       </c>
     </row>
@@ -1938,11 +1968,12 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="1">
     <mergeCell ref="A44:B44"/>
   </mergeCells>
   <printOptions horizontalCentered="1" gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup fitToHeight="0" pageOrder="overThenDown" orientation="landscape" cellComments="atEnd"/>
+  <pageSetup fitToHeight="0" pageOrder="overThenDown" orientation="landscape" cellComments="atEnd" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added example student specific data in the xlsx file
</commit_message>
<xml_diff>
--- a/src/FormatForTemplateOfScores.xlsx
+++ b/src/FormatForTemplateOfScores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harle\Documents\mySourceCode\react\wiat-4CustomReportGenerator\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4DFC05A-C214-420C-A306-71DEAA287995}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD52EC0B-B0D2-426E-88A1-F8B03EAD32F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="87">
   <si>
     <t>Student Name:</t>
   </si>
@@ -174,6 +174,117 @@
    • Recomendation list item #1
    • Recomendation list item #2
    • Recomendation list item #3</t>
+  </si>
+  <si>
+    <t>Student Specific Information for the Oral Language Composite</t>
+  </si>
+  <si>
+    <t>Student Specific Information for the Phonological Processing Composite</t>
+  </si>
+  <si>
+    <t>Student Specific Information for the Orthographic Processing Composite</t>
+  </si>
+  <si>
+    <t>Student Specific Information for the Orthographic Fluency subtest</t>
+  </si>
+  <si>
+    <t>Student Specific Information for the Spelling subtest</t>
+  </si>
+  <si>
+    <t>Student Specific Information for the Receptive Vocabulary subtest</t>
+  </si>
+  <si>
+    <t>Student Specific Information for the Listening Comprehension subtest</t>
+  </si>
+  <si>
+    <t>Student Specific Information for the Oral Discourse Comprehension</t>
+  </si>
+  <si>
+    <t>Student Specific Information for the Oral Expression subtest</t>
+  </si>
+  <si>
+    <t>Student Specific Information for the Expressive Vocabulary subtest</t>
+  </si>
+  <si>
+    <t>Student Specific Information for the Oral Word Fluency subtest</t>
+  </si>
+  <si>
+    <t>Student Specific Information for the Sentence Repetition subtest</t>
+  </si>
+  <si>
+    <t>Student Specific Information for the Pseudoword Decoding subtest</t>
+  </si>
+  <si>
+    <t>Student Specific Information for Phonemic Proficiency subtest</t>
+  </si>
+  <si>
+    <t>Student Specific Information for the Orthographic Choice subtest</t>
+  </si>
+  <si>
+    <t>Student Specific Information for the Reading Composite</t>
+  </si>
+  <si>
+    <t>Student Specific Information for the Word Reading subtest</t>
+  </si>
+  <si>
+    <t>Student Specific Information for the Reading Comprehension subtest</t>
+  </si>
+  <si>
+    <t>Student Specific Information for the Basic Reading (and Decoding) Composite</t>
+  </si>
+  <si>
+    <t>Student Specific Information for the Reading Fluency Composite</t>
+  </si>
+  <si>
+    <t>Student Specific Information for the Oral Reading Fluency subtest</t>
+  </si>
+  <si>
+    <t>Student Specific Information for the Decoding Fluency subtest</t>
+  </si>
+  <si>
+    <t>Student Specific Information for the Written Expression Composite</t>
+  </si>
+  <si>
+    <t>Student Specific Information for the Sentence Composition subtest</t>
+  </si>
+  <si>
+    <t>Student Specific Information for the Essay Composition subtest</t>
+  </si>
+  <si>
+    <t>Student Specific Information for the Sentence Building subtest</t>
+  </si>
+  <si>
+    <t>Student Specific Information for the Sentence Combining subtest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Student Specific Information for the Writing Fluency composite </t>
+  </si>
+  <si>
+    <t>Student Specific Information for Alphabet Writing Fluency subtest</t>
+  </si>
+  <si>
+    <t>Student Specific Information for Sentence Writing Fluency subtest</t>
+  </si>
+  <si>
+    <t>Student Specific Information for the Mathematics Composite</t>
+  </si>
+  <si>
+    <t>Student Specific Information for the Math Problem Solving subtest</t>
+  </si>
+  <si>
+    <t>Student Specific Information for the Numerical Operations subtest</t>
+  </si>
+  <si>
+    <t>Student Specific Information for the Math Fluency Composite</t>
+  </si>
+  <si>
+    <t>Student Specific Information for the Math Fluency–Addition subtest</t>
+  </si>
+  <si>
+    <t>Student Specific Information for the Math Fluency–Subtraction subtest</t>
+  </si>
+  <si>
+    <t>Student Specific Information for Math Fluency–Multiplication subtest</t>
   </si>
 </sst>
 </file>
@@ -386,10 +497,6 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -400,6 +507,10 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -622,7 +733,7 @@
   <dimension ref="A1:C43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
@@ -632,7 +743,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -640,7 +751,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="13" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -648,7 +759,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="13" t="s">
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -659,24 +770,26 @@
       </c>
     </row>
     <row r="4" spans="1:3" ht="38.25" customHeight="1">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="12" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.75" customHeight="1">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="13">
+      <c r="B5" s="11">
         <v>73</v>
       </c>
-      <c r="C5" s="4"/>
+      <c r="C5" s="4" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="6" spans="1:3" ht="15">
       <c r="A6" s="5" t="s">
@@ -685,7 +798,9 @@
       <c r="B6" s="3">
         <v>73</v>
       </c>
-      <c r="C6" s="4"/>
+      <c r="C6" s="4" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="7" spans="1:3" ht="15">
       <c r="A7" s="5" t="s">
@@ -694,7 +809,9 @@
       <c r="B7" s="3">
         <v>75</v>
       </c>
-      <c r="C7" s="6"/>
+      <c r="C7" s="4" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="8" spans="1:3" ht="15">
       <c r="A8" s="5" t="s">
@@ -703,7 +820,9 @@
       <c r="B8" s="3">
         <v>79</v>
       </c>
-      <c r="C8" s="6"/>
+      <c r="C8" s="4" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="9" spans="1:3" ht="15">
       <c r="A9" s="5" t="s">
@@ -712,7 +831,9 @@
       <c r="B9" s="3">
         <v>76</v>
       </c>
-      <c r="C9" s="4"/>
+      <c r="C9" s="4" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="10" spans="1:3" ht="15">
       <c r="A10" s="5" t="s">
@@ -721,7 +842,9 @@
       <c r="B10" s="3">
         <v>75</v>
       </c>
-      <c r="C10" s="4"/>
+      <c r="C10" s="4" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="11" spans="1:3" ht="15">
       <c r="A11" s="5" t="s">
@@ -730,7 +853,9 @@
       <c r="B11" s="3">
         <v>96</v>
       </c>
-      <c r="C11" s="4"/>
+      <c r="C11" s="4" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="12" spans="1:3" ht="15">
       <c r="A12" s="5" t="s">
@@ -739,7 +864,9 @@
       <c r="B12" s="3">
         <v>70</v>
       </c>
-      <c r="C12" s="4"/>
+      <c r="C12" s="4" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="13" spans="1:3" ht="15.75" customHeight="1">
       <c r="A13" s="7" t="s">
@@ -748,7 +875,9 @@
       <c r="B13" s="8">
         <v>89</v>
       </c>
-      <c r="C13" s="4"/>
+      <c r="C13" s="4" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="14" spans="1:3" ht="15">
       <c r="A14" s="9" t="s">
@@ -757,7 +886,9 @@
       <c r="B14" s="8">
         <v>97</v>
       </c>
-      <c r="C14" s="4"/>
+      <c r="C14" s="4" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="15" spans="1:3" ht="15">
       <c r="A15" s="9" t="s">
@@ -766,7 +897,9 @@
       <c r="B15" s="8">
         <v>85</v>
       </c>
-      <c r="C15" s="4"/>
+      <c r="C15" s="4" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="16" spans="1:3" ht="15.75" customHeight="1">
       <c r="A16" s="2" t="s">
@@ -775,7 +908,9 @@
       <c r="B16" s="3">
         <v>79</v>
       </c>
-      <c r="C16" s="4"/>
+      <c r="C16" s="4" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="17" spans="1:3" ht="15">
       <c r="A17" s="5" t="s">
@@ -784,7 +919,9 @@
       <c r="B17" s="3">
         <v>77</v>
       </c>
-      <c r="C17" s="4"/>
+      <c r="C17" s="4" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="18" spans="1:3" ht="15">
       <c r="A18" s="5" t="s">
@@ -793,7 +930,9 @@
       <c r="B18" s="3">
         <v>79</v>
       </c>
-      <c r="C18" s="4"/>
+      <c r="C18" s="4" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="19" spans="1:3" ht="15">
       <c r="A19" s="5" t="s">
@@ -802,7 +941,9 @@
       <c r="B19" s="3">
         <v>88</v>
       </c>
-      <c r="C19" s="4"/>
+      <c r="C19" s="4" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="20" spans="1:3" ht="15.75" customHeight="1">
       <c r="A20" s="7" t="s">
@@ -811,7 +952,9 @@
       <c r="B20" s="8">
         <v>81</v>
       </c>
-      <c r="C20" s="4"/>
+      <c r="C20" s="4" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="21" spans="1:3" ht="15">
       <c r="A21" s="9" t="s">
@@ -820,7 +963,9 @@
       <c r="B21" s="8">
         <v>82</v>
       </c>
-      <c r="C21" s="4"/>
+      <c r="C21" s="4" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="22" spans="1:3" ht="15">
       <c r="A22" s="9" t="s">
@@ -829,7 +974,9 @@
       <c r="B22" s="8">
         <v>85</v>
       </c>
-      <c r="C22" s="4"/>
+      <c r="C22" s="4" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="23" spans="1:3" ht="15.75" customHeight="1">
       <c r="A23" s="2" t="s">
@@ -838,7 +985,9 @@
       <c r="B23" s="3">
         <v>86</v>
       </c>
-      <c r="C23" s="4"/>
+      <c r="C23" s="4" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="24" spans="1:3" ht="15.75" customHeight="1">
       <c r="A24" s="7" t="s">
@@ -847,7 +996,9 @@
       <c r="B24" s="8">
         <v>101</v>
       </c>
-      <c r="C24" s="4"/>
+      <c r="C24" s="4" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="25" spans="1:3" ht="15">
       <c r="A25" s="9" t="s">
@@ -856,7 +1007,9 @@
       <c r="B25" s="8">
         <v>134</v>
       </c>
-      <c r="C25" s="4"/>
+      <c r="C25" s="4" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="26" spans="1:3" ht="15">
       <c r="A26" s="9" t="s">
@@ -865,7 +1018,9 @@
       <c r="B26" s="8">
         <v>93</v>
       </c>
-      <c r="C26" s="4"/>
+      <c r="C26" s="4" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="27" spans="1:3" ht="15.75" customHeight="1">
       <c r="A27" s="2" t="s">
@@ -874,7 +1029,9 @@
       <c r="B27" s="3">
         <v>80</v>
       </c>
-      <c r="C27" s="4"/>
+      <c r="C27" s="4" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="28" spans="1:3" ht="15">
       <c r="A28" s="5" t="s">
@@ -883,7 +1040,9 @@
       <c r="B28" s="3">
         <v>92</v>
       </c>
-      <c r="C28" s="4"/>
+      <c r="C28" s="4" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="29" spans="1:3" ht="15">
       <c r="A29" s="5" t="s">
@@ -892,7 +1051,9 @@
       <c r="B29" s="3">
         <v>81</v>
       </c>
-      <c r="C29" s="4"/>
+      <c r="C29" s="4" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="30" spans="1:3" ht="15">
       <c r="A30" s="5" t="s">
@@ -901,7 +1062,9 @@
       <c r="B30" s="3">
         <v>93</v>
       </c>
-      <c r="C30" s="4"/>
+      <c r="C30" s="4" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="31" spans="1:3" ht="15">
       <c r="A31" s="5" t="s">
@@ -910,7 +1073,9 @@
       <c r="B31" s="3">
         <v>95</v>
       </c>
-      <c r="C31" s="4"/>
+      <c r="C31" s="4" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="32" spans="1:3" ht="15.75" customHeight="1">
       <c r="A32" s="7" t="s">
@@ -919,7 +1084,9 @@
       <c r="B32" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C32" s="4"/>
+      <c r="C32" s="4" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="33" spans="1:3" ht="15">
       <c r="A33" s="9" t="s">
@@ -928,7 +1095,9 @@
       <c r="B33" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C33" s="4"/>
+      <c r="C33" s="4" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="34" spans="1:3" ht="15">
       <c r="A34" s="9" t="s">
@@ -937,7 +1106,9 @@
       <c r="B34" s="8">
         <v>82</v>
       </c>
-      <c r="C34" s="4"/>
+      <c r="C34" s="4" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="35" spans="1:3" ht="15.75" customHeight="1">
       <c r="A35" s="2" t="s">
@@ -946,7 +1117,9 @@
       <c r="B35" s="3">
         <v>67</v>
       </c>
-      <c r="C35" s="4"/>
+      <c r="C35" s="4" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="36" spans="1:3" ht="15">
       <c r="A36" s="5" t="s">
@@ -955,7 +1128,9 @@
       <c r="B36" s="3">
         <v>68</v>
       </c>
-      <c r="C36" s="4"/>
+      <c r="C36" s="4" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="37" spans="1:3" ht="15">
       <c r="A37" s="5" t="s">
@@ -964,7 +1139,9 @@
       <c r="B37" s="3">
         <v>71</v>
       </c>
-      <c r="C37" s="4"/>
+      <c r="C37" s="4" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="38" spans="1:3">
       <c r="A38" s="7" t="s">
@@ -973,7 +1150,9 @@
       <c r="B38" s="8">
         <v>70</v>
       </c>
-      <c r="C38" s="4"/>
+      <c r="C38" s="4" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="39" spans="1:3" ht="15">
       <c r="A39" s="9" t="s">
@@ -982,7 +1161,9 @@
       <c r="B39" s="8">
         <v>76</v>
       </c>
-      <c r="C39" s="4"/>
+      <c r="C39" s="4" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="40" spans="1:3" ht="15">
       <c r="A40" s="9" t="s">
@@ -991,7 +1172,9 @@
       <c r="B40" s="8">
         <v>71</v>
       </c>
-      <c r="C40" s="4"/>
+      <c r="C40" s="4" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="41" spans="1:3" ht="15">
       <c r="A41" s="9" t="s">
@@ -1000,13 +1183,15 @@
       <c r="B41" s="8">
         <v>72</v>
       </c>
-      <c r="C41" s="4"/>
+      <c r="C41" s="4" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="43" spans="1:3" ht="178.5">
-      <c r="A43" s="10" t="s">
+      <c r="A43" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="B43" s="11"/>
+      <c r="B43" s="15"/>
       <c r="C43" s="6" t="s">
         <v>49</v>
       </c>

</xml_diff>

<commit_message>
subtest added (alphabet writing fluency); fix made allowins commas in student specific info; fix to example template (can be opened now in google sheets or excel with pretty colors/spaces
</commit_message>
<xml_diff>
--- a/src/FormatForTemplateOfScores.xlsx
+++ b/src/FormatForTemplateOfScores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\harle\Documents\mySourceCode\react\wiat-4CustomReportGenerator\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD52EC0B-B0D2-426E-88A1-F8B03EAD32F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3BA3D07-B895-4723-B8CA-063F2BA314B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -169,122 +169,122 @@
     <t>Conclusions:</t>
   </si>
   <si>
-    <t>This is where we can place all of our conclusions about Student-Name's performance on the exam. This way, this single CSV file will contain all of the important results of the student at-a-glance, which I have been told will be a very useful document for the Special Education Teacher as before a meeting, the teacher can look at all of the information in one place (especially when they have so many students on their caseload), which is excellent, as any functionality which will improve the work-flow of a teacher, or simply improve the quality of work-life of a teacher, is certainly worth the (minor) efforts to include this functionality in the report generator!  With Word Wrapping on a cell, the conclusion can be very readable indeed within a spreadsheet application! Now, all of the student specific data and all of the teacher's observations/recordings are in one single document; quite glorious indeed!
-We can even add a bulleted list into this conclusion (but it will currently appear as inline text in the generated report). Example: The following list presents my recomendations based on this test for Student-Name:
+    <t>Student Specific Information for Sentence Writing Fluency subtest.</t>
+  </si>
+  <si>
+    <t>Student Specific Information for the Mathematics Composite.</t>
+  </si>
+  <si>
+    <t>Student Specific Information for the Math Problem Solving subtest.</t>
+  </si>
+  <si>
+    <t>Student Specific Information for the Numerical Operations subtest.</t>
+  </si>
+  <si>
+    <t>Student Specific Information for the Math Fluency Composite.</t>
+  </si>
+  <si>
+    <t>Student Specific Information for the Math Fluency–Addition subtest.</t>
+  </si>
+  <si>
+    <t>Student Specific Information for the Math Fluency–Subtraction subtest.</t>
+  </si>
+  <si>
+    <t>Student Specific Information for Math Fluency–Multiplication subtest.</t>
+  </si>
+  <si>
+    <t>Student Specific Information for the Writing Fluency composite.</t>
+  </si>
+  <si>
+    <t>Student Specific Information for the Sentence Combining subtest.</t>
+  </si>
+  <si>
+    <t>Student Specific Information for the Sentence Building subtest.</t>
+  </si>
+  <si>
+    <t>Student Specific Information for the Essay Composition subtest.</t>
+  </si>
+  <si>
+    <t>Student Specific Information for the Sentence Composition subtest.</t>
+  </si>
+  <si>
+    <t>Student Specific Information for the Written Expression Composite.</t>
+  </si>
+  <si>
+    <t>Student Specific Information for the Decoding Fluency subtest.</t>
+  </si>
+  <si>
+    <t>Student Specific Information for the Oral Reading Fluency subtest.</t>
+  </si>
+  <si>
+    <t>Student Specific Information for the Reading Fluency Composite.</t>
+  </si>
+  <si>
+    <t>Student Specific Information for the Basic Reading (and Decoding) Composite.</t>
+  </si>
+  <si>
+    <t>Student Specific Information for the Reading Comprehension subtest.</t>
+  </si>
+  <si>
+    <t>Student Specific Information for the Word Reading subtest.</t>
+  </si>
+  <si>
+    <t>Student Specific Information for the Reading Composite.</t>
+  </si>
+  <si>
+    <t>Student Specific Information for the Orthographic Choice subtest.</t>
+  </si>
+  <si>
+    <t>Student Specific Information for the Spelling subtest.</t>
+  </si>
+  <si>
+    <t>Student Specific Information for the Orthographic Fluency subtest.</t>
+  </si>
+  <si>
+    <t>Student Specific Information for the Orthographic Processing Composite.</t>
+  </si>
+  <si>
+    <t>Student Specific Information for Phonemic Proficiency subtest.</t>
+  </si>
+  <si>
+    <t>Student Specific Information for the Pseudoword Decoding subtest.</t>
+  </si>
+  <si>
+    <t>Student Specific Information for the Phonological Processing Composite.</t>
+  </si>
+  <si>
+    <t>Student Specific Information for the Sentence Repetition subtest.</t>
+  </si>
+  <si>
+    <t>Student Specific Information for the Oral Word Fluency subtest.</t>
+  </si>
+  <si>
+    <t>Student Specific Information for the Expressive Vocabulary subtest.</t>
+  </si>
+  <si>
+    <t>Student Specific Information for the Oral Expression subtest.</t>
+  </si>
+  <si>
+    <t>Student Specific Information for the Oral Discourse Comprehension.</t>
+  </si>
+  <si>
+    <t>Student Specific Information for the Receptive Vocabulary subtest.</t>
+  </si>
+  <si>
+    <t>Student Specific Information for the Listening Comprehension subtest.</t>
+  </si>
+  <si>
+    <t>Student Specific Information for the Oral Language Composite.</t>
+  </si>
+  <si>
+    <t>This is where we can place all of our conclusions about Student-Name's performance on the exam. This way, this single CSV file will contain all of the important results of the student at-a-glance, which I have been told will be a very useful document for the Special Education Teacher as before a meeting, the teacher can look at all of the information in one place (especially when they have so many students on their caseload), which is excellent, as any functionality which will improve the work-flow of a teacher, or simply improve the quality of work-life of a teacher, is certainly worth the (minor) efforts to include this functionality in the report generator.  With Word Wrapping on a cell, the conclusion can be very readable indeed within a spreadsheet application. With this addition of adding concluding remarks, all of the student specific data and all of the teacher's observations/recordings are in one single document; quite glorious indeed!
+We can even add a bulleted list into this conclusion (a copy/paste of a bullet symbol is required). Example: The following list presents my recomendations based on this test for Student-Name:
    • Recomendation list item #1
    • Recomendation list item #2
    • Recomendation list item #3</t>
   </si>
   <si>
-    <t>Student Specific Information for the Oral Language Composite</t>
-  </si>
-  <si>
-    <t>Student Specific Information for the Phonological Processing Composite</t>
-  </si>
-  <si>
-    <t>Student Specific Information for the Orthographic Processing Composite</t>
-  </si>
-  <si>
-    <t>Student Specific Information for the Orthographic Fluency subtest</t>
-  </si>
-  <si>
-    <t>Student Specific Information for the Spelling subtest</t>
-  </si>
-  <si>
-    <t>Student Specific Information for the Receptive Vocabulary subtest</t>
-  </si>
-  <si>
-    <t>Student Specific Information for the Listening Comprehension subtest</t>
-  </si>
-  <si>
-    <t>Student Specific Information for the Oral Discourse Comprehension</t>
-  </si>
-  <si>
-    <t>Student Specific Information for the Oral Expression subtest</t>
-  </si>
-  <si>
-    <t>Student Specific Information for the Expressive Vocabulary subtest</t>
-  </si>
-  <si>
-    <t>Student Specific Information for the Oral Word Fluency subtest</t>
-  </si>
-  <si>
-    <t>Student Specific Information for the Sentence Repetition subtest</t>
-  </si>
-  <si>
-    <t>Student Specific Information for the Pseudoword Decoding subtest</t>
-  </si>
-  <si>
-    <t>Student Specific Information for Phonemic Proficiency subtest</t>
-  </si>
-  <si>
-    <t>Student Specific Information for the Orthographic Choice subtest</t>
-  </si>
-  <si>
-    <t>Student Specific Information for the Reading Composite</t>
-  </si>
-  <si>
-    <t>Student Specific Information for the Word Reading subtest</t>
-  </si>
-  <si>
-    <t>Student Specific Information for the Reading Comprehension subtest</t>
-  </si>
-  <si>
-    <t>Student Specific Information for the Basic Reading (and Decoding) Composite</t>
-  </si>
-  <si>
-    <t>Student Specific Information for the Reading Fluency Composite</t>
-  </si>
-  <si>
-    <t>Student Specific Information for the Oral Reading Fluency subtest</t>
-  </si>
-  <si>
-    <t>Student Specific Information for the Decoding Fluency subtest</t>
-  </si>
-  <si>
-    <t>Student Specific Information for the Written Expression Composite</t>
-  </si>
-  <si>
-    <t>Student Specific Information for the Sentence Composition subtest</t>
-  </si>
-  <si>
-    <t>Student Specific Information for the Essay Composition subtest</t>
-  </si>
-  <si>
-    <t>Student Specific Information for the Sentence Building subtest</t>
-  </si>
-  <si>
-    <t>Student Specific Information for the Sentence Combining subtest</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Student Specific Information for the Writing Fluency composite </t>
-  </si>
-  <si>
-    <t>Student Specific Information for Alphabet Writing Fluency subtest</t>
-  </si>
-  <si>
-    <t>Student Specific Information for Sentence Writing Fluency subtest</t>
-  </si>
-  <si>
-    <t>Student Specific Information for the Mathematics Composite</t>
-  </si>
-  <si>
-    <t>Student Specific Information for the Math Problem Solving subtest</t>
-  </si>
-  <si>
-    <t>Student Specific Information for the Numerical Operations subtest</t>
-  </si>
-  <si>
-    <t>Student Specific Information for the Math Fluency Composite</t>
-  </si>
-  <si>
-    <t>Student Specific Information for the Math Fluency–Addition subtest</t>
-  </si>
-  <si>
-    <t>Student Specific Information for the Math Fluency–Subtraction subtest</t>
-  </si>
-  <si>
-    <t>Student Specific Information for Math Fluency–Multiplication subtest</t>
+    <t>Student Name did not have the Alphabet Writing Fluency subtest administered because, [insert description here].</t>
   </si>
 </sst>
 </file>
@@ -732,8 +732,8 @@
   </sheetPr>
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
@@ -788,7 +788,7 @@
         <v>73</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>50</v>
+        <v>84</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15">
@@ -799,7 +799,7 @@
         <v>73</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>56</v>
+        <v>83</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15">
@@ -810,7 +810,7 @@
         <v>75</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>55</v>
+        <v>82</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="15">
@@ -821,7 +821,7 @@
         <v>79</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>57</v>
+        <v>81</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15">
@@ -832,7 +832,7 @@
         <v>76</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>58</v>
+        <v>80</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="15">
@@ -843,7 +843,7 @@
         <v>75</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>59</v>
+        <v>79</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="15">
@@ -854,7 +854,7 @@
         <v>96</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>60</v>
+        <v>78</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="15">
@@ -865,7 +865,7 @@
         <v>70</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>61</v>
+        <v>77</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="15.75" customHeight="1">
@@ -876,7 +876,7 @@
         <v>89</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>51</v>
+        <v>76</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="15">
@@ -887,7 +887,7 @@
         <v>97</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>62</v>
+        <v>75</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="15">
@@ -898,7 +898,7 @@
         <v>85</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>63</v>
+        <v>74</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="15.75" customHeight="1">
@@ -909,7 +909,7 @@
         <v>79</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>52</v>
+        <v>73</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="15">
@@ -920,7 +920,7 @@
         <v>77</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>53</v>
+        <v>72</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="15">
@@ -931,7 +931,7 @@
         <v>79</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>54</v>
+        <v>71</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="15">
@@ -942,7 +942,7 @@
         <v>88</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="15.75" customHeight="1">
@@ -953,7 +953,7 @@
         <v>81</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="15">
@@ -964,7 +964,7 @@
         <v>82</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="15">
@@ -986,7 +986,7 @@
         <v>86</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="15.75" customHeight="1">
@@ -997,7 +997,7 @@
         <v>101</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="15">
@@ -1008,7 +1008,7 @@
         <v>134</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="15">
@@ -1019,7 +1019,7 @@
         <v>93</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="15.75" customHeight="1">
@@ -1030,7 +1030,7 @@
         <v>80</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="15">
@@ -1041,7 +1041,7 @@
         <v>92</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="15">
@@ -1052,7 +1052,7 @@
         <v>81</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="15">
@@ -1063,7 +1063,7 @@
         <v>93</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="15">
@@ -1074,7 +1074,7 @@
         <v>95</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>76</v>
+        <v>58</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="15.75" customHeight="1">
@@ -1085,7 +1085,7 @@
         <v>38</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>77</v>
+        <v>57</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="15">
@@ -1096,7 +1096,7 @@
         <v>38</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="15">
@@ -1107,7 +1107,7 @@
         <v>82</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>79</v>
+        <v>49</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="15.75" customHeight="1">
@@ -1118,7 +1118,7 @@
         <v>67</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>80</v>
+        <v>50</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="15">
@@ -1129,7 +1129,7 @@
         <v>68</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>81</v>
+        <v>51</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="15">
@@ -1140,7 +1140,7 @@
         <v>71</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>82</v>
+        <v>52</v>
       </c>
     </row>
     <row r="38" spans="1:3">
@@ -1151,7 +1151,7 @@
         <v>70</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>83</v>
+        <v>53</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="15">
@@ -1162,7 +1162,7 @@
         <v>76</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>84</v>
+        <v>54</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="15">
@@ -1173,7 +1173,7 @@
         <v>71</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>85</v>
+        <v>55</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="15">
@@ -1184,7 +1184,7 @@
         <v>72</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>86</v>
+        <v>56</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="178.5">
@@ -1193,7 +1193,7 @@
       </c>
       <c r="B43" s="15"/>
       <c r="C43" s="6" t="s">
-        <v>49</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>